<commit_message>
9 working sceneraios for user
</commit_message>
<xml_diff>
--- a/Doc/Project plan.xlsx
+++ b/Doc/Project plan.xlsx
@@ -632,7 +632,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="69">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -797,10 +797,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -809,15 +805,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -845,10 +833,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -887,10 +871,6 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1011,15 +991,15 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="Y36" activeCellId="0" sqref="Y36"/>
+      <selection pane="bottomLeft" activeCell="AJ28" activeCellId="0" sqref="AJ28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="67.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="4" style="0" width="3.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="67.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="4" style="0" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="4.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1010" min="59" style="0" width="17.33"/>
@@ -1730,11 +1710,11 @@
       <c r="U11" s="40"/>
       <c r="V11" s="40"/>
       <c r="W11" s="40"/>
-      <c r="X11" s="41"/>
-      <c r="Y11" s="41"/>
-      <c r="Z11" s="41"/>
-      <c r="AA11" s="41"/>
-      <c r="AB11" s="41"/>
+      <c r="X11" s="36"/>
+      <c r="Y11" s="36"/>
+      <c r="Z11" s="36"/>
+      <c r="AA11" s="36"/>
+      <c r="AB11" s="36"/>
       <c r="AC11" s="36"/>
       <c r="AD11" s="36"/>
       <c r="AE11" s="36"/>
@@ -1769,11 +1749,11 @@
       <c r="B12" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
+      <c r="C12" s="41"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
       <c r="M12" s="39"/>
       <c r="N12" s="39"/>
       <c r="O12" s="14"/>
@@ -1785,192 +1765,171 @@
       <c r="U12" s="40"/>
       <c r="V12" s="40"/>
       <c r="W12" s="40"/>
-      <c r="X12" s="44"/>
-      <c r="Y12" s="44"/>
-      <c r="Z12" s="44"/>
-      <c r="AA12" s="44"/>
-      <c r="AB12" s="44"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32"/>
       <c r="B13" s="25"/>
-      <c r="C13" s="42"/>
+      <c r="C13" s="41"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32"/>
       <c r="B14" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="45"/>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="45"/>
-      <c r="R14" s="45"/>
-      <c r="S14" s="45"/>
-      <c r="T14" s="45"/>
-      <c r="U14" s="45"/>
-      <c r="V14" s="45"/>
-      <c r="W14" s="45"/>
-      <c r="X14" s="45"/>
-      <c r="Y14" s="45"/>
-      <c r="Z14" s="45"/>
-      <c r="AA14" s="45"/>
-      <c r="AB14" s="45"/>
-      <c r="AC14" s="45"/>
-      <c r="AD14" s="45"/>
-      <c r="AE14" s="45"/>
-      <c r="AF14" s="45"/>
-      <c r="AG14" s="45"/>
-      <c r="AH14" s="45"/>
-      <c r="AI14" s="45"/>
-      <c r="AJ14" s="45"/>
-      <c r="AK14" s="45"/>
-      <c r="AL14" s="45"/>
-      <c r="AM14" s="45"/>
-      <c r="AN14" s="45"/>
-      <c r="AO14" s="45"/>
-      <c r="AP14" s="45"/>
-      <c r="AQ14" s="45"/>
-      <c r="AR14" s="45"/>
-      <c r="AS14" s="45"/>
-      <c r="AT14" s="45"/>
-      <c r="AU14" s="45"/>
-      <c r="AV14" s="45"/>
-      <c r="AW14" s="45"/>
-      <c r="AX14" s="45"/>
-      <c r="AY14" s="45"/>
-      <c r="AZ14" s="45"/>
-      <c r="BA14" s="45"/>
-      <c r="BB14" s="45"/>
-      <c r="BC14" s="45"/>
-      <c r="BD14" s="45"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="43"/>
+      <c r="T14" s="43"/>
+      <c r="U14" s="43"/>
+      <c r="V14" s="43"/>
+      <c r="W14" s="43"/>
+      <c r="X14" s="43"/>
+      <c r="Y14" s="43"/>
+      <c r="Z14" s="43"/>
+      <c r="AA14" s="43"/>
+      <c r="AB14" s="43"/>
+      <c r="AC14" s="43"/>
+      <c r="AD14" s="43"/>
+      <c r="AE14" s="43"/>
+      <c r="AF14" s="43"/>
+      <c r="AG14" s="43"/>
+      <c r="AH14" s="43"/>
+      <c r="AI14" s="43"/>
+      <c r="AJ14" s="43"/>
+      <c r="AK14" s="43"/>
+      <c r="AL14" s="43"/>
+      <c r="AM14" s="43"/>
+      <c r="AN14" s="43"/>
+      <c r="AO14" s="43"/>
+      <c r="AP14" s="43"/>
+      <c r="AQ14" s="43"/>
+      <c r="AR14" s="43"/>
+      <c r="AS14" s="43"/>
+      <c r="AT14" s="43"/>
+      <c r="AU14" s="43"/>
+      <c r="AV14" s="43"/>
+      <c r="AW14" s="43"/>
+      <c r="AX14" s="43"/>
+      <c r="AY14" s="43"/>
+      <c r="AZ14" s="43"/>
+      <c r="BA14" s="43"/>
+      <c r="BB14" s="43"/>
+      <c r="BC14" s="43"/>
+      <c r="BD14" s="43"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="32"/>
       <c r="B15" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="42"/>
+      <c r="C15" s="41"/>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
-      <c r="T15" s="46"/>
-      <c r="U15" s="46"/>
-      <c r="AE15" s="44"/>
-      <c r="AF15" s="44"/>
-      <c r="AG15" s="43"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
+      <c r="AG15" s="42"/>
       <c r="AH15" s="40"/>
-      <c r="AI15" s="43"/>
-      <c r="AJ15" s="43"/>
-      <c r="AK15" s="43"/>
-      <c r="AL15" s="43"/>
-      <c r="AM15" s="43"/>
-      <c r="AN15" s="43"/>
-      <c r="AO15" s="43"/>
-      <c r="AP15" s="43"/>
-      <c r="AQ15" s="43"/>
-      <c r="AR15" s="47"/>
-      <c r="AS15" s="47"/>
-      <c r="AT15" s="47"/>
-      <c r="AU15" s="47"/>
-      <c r="AV15" s="47"/>
-      <c r="AW15" s="47"/>
-      <c r="AX15" s="47"/>
+      <c r="AI15" s="42"/>
+      <c r="AJ15" s="42"/>
+      <c r="AK15" s="42"/>
+      <c r="AL15" s="42"/>
+      <c r="AM15" s="42"/>
+      <c r="AN15" s="42"/>
+      <c r="AO15" s="42"/>
+      <c r="AP15" s="42"/>
+      <c r="AQ15" s="42"/>
+      <c r="AR15" s="44"/>
+      <c r="AS15" s="44"/>
+      <c r="AT15" s="44"/>
+      <c r="AU15" s="44"/>
+      <c r="AV15" s="44"/>
+      <c r="AW15" s="44"/>
+      <c r="AX15" s="44"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="32"/>
       <c r="B16" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="48"/>
+      <c r="C16" s="45"/>
       <c r="D16" s="25"/>
       <c r="E16" s="25"/>
-      <c r="T16" s="46"/>
-      <c r="U16" s="46"/>
-      <c r="AE16" s="44"/>
-      <c r="AF16" s="44"/>
-      <c r="AG16" s="43"/>
-      <c r="AH16" s="49"/>
+      <c r="T16" s="40"/>
+      <c r="U16" s="40"/>
+      <c r="AG16" s="42"/>
+      <c r="AH16" s="46"/>
       <c r="AI16" s="39"/>
-      <c r="AJ16" s="47"/>
-      <c r="AK16" s="44"/>
-      <c r="AL16" s="44"/>
-      <c r="AM16" s="44"/>
-      <c r="AN16" s="43"/>
-      <c r="AO16" s="43"/>
-      <c r="AP16" s="43"/>
-      <c r="AQ16" s="43"/>
-      <c r="AR16" s="44"/>
-      <c r="AS16" s="47"/>
-      <c r="AT16" s="47"/>
-      <c r="AU16" s="47"/>
-      <c r="AV16" s="47"/>
-      <c r="AW16" s="47"/>
-      <c r="AX16" s="44"/>
+      <c r="AJ16" s="44"/>
+      <c r="AN16" s="42"/>
+      <c r="AO16" s="42"/>
+      <c r="AP16" s="42"/>
+      <c r="AQ16" s="42"/>
+      <c r="AS16" s="44"/>
+      <c r="AT16" s="44"/>
+      <c r="AU16" s="44"/>
+      <c r="AV16" s="44"/>
+      <c r="AW16" s="44"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="32"/>
       <c r="B17" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="S17" s="44"/>
-      <c r="AE17" s="44"/>
-      <c r="AF17" s="44"/>
-      <c r="AG17" s="43"/>
+      <c r="C17" s="47"/>
+      <c r="AG17" s="42"/>
       <c r="AH17" s="19"/>
       <c r="AI17" s="19"/>
-      <c r="AJ17" s="43"/>
+      <c r="AJ17" s="42"/>
       <c r="AK17" s="39"/>
       <c r="AL17" s="39"/>
-      <c r="AM17" s="47"/>
-      <c r="AN17" s="47"/>
-      <c r="AO17" s="47"/>
-      <c r="AP17" s="47"/>
-      <c r="AQ17" s="47"/>
-      <c r="AR17" s="47"/>
-      <c r="AS17" s="47"/>
-      <c r="AT17" s="47"/>
-      <c r="AU17" s="47"/>
-      <c r="AV17" s="47"/>
-      <c r="AW17" s="47"/>
-      <c r="AX17" s="44"/>
+      <c r="AM17" s="44"/>
+      <c r="AN17" s="44"/>
+      <c r="AO17" s="44"/>
+      <c r="AP17" s="44"/>
+      <c r="AQ17" s="44"/>
+      <c r="AR17" s="44"/>
+      <c r="AS17" s="44"/>
+      <c r="AT17" s="44"/>
+      <c r="AU17" s="44"/>
+      <c r="AV17" s="44"/>
+      <c r="AW17" s="44"/>
     </row>
     <row r="18" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="32"/>
       <c r="B18" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="S18" s="43"/>
-      <c r="T18" s="44"/>
-      <c r="AE18" s="44"/>
-      <c r="AF18" s="44"/>
-      <c r="AG18" s="43"/>
-      <c r="AH18" s="43"/>
-      <c r="AI18" s="43"/>
-      <c r="AJ18" s="43"/>
+      <c r="C18" s="47"/>
+      <c r="S18" s="42"/>
+      <c r="AG18" s="42"/>
+      <c r="AH18" s="42"/>
+      <c r="AI18" s="42"/>
+      <c r="AJ18" s="42"/>
       <c r="AK18" s="19"/>
-      <c r="AL18" s="43"/>
-      <c r="AM18" s="47"/>
-      <c r="AN18" s="47"/>
-      <c r="AO18" s="47"/>
-      <c r="AP18" s="47"/>
-      <c r="AQ18" s="47"/>
-      <c r="AR18" s="47"/>
-      <c r="AS18" s="47"/>
-      <c r="AT18" s="47"/>
-      <c r="AU18" s="51"/>
+      <c r="AL18" s="42"/>
+      <c r="AM18" s="44"/>
+      <c r="AN18" s="44"/>
+      <c r="AO18" s="44"/>
+      <c r="AP18" s="44"/>
+      <c r="AQ18" s="44"/>
+      <c r="AR18" s="44"/>
+      <c r="AS18" s="44"/>
+      <c r="AT18" s="44"/>
+      <c r="AU18" s="48"/>
       <c r="AV18" s="14"/>
       <c r="AW18" s="14"/>
       <c r="AX18" s="40"/>
@@ -1980,333 +1939,270 @@
       <c r="B19" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="S19" s="43"/>
-      <c r="T19" s="44"/>
-      <c r="AE19" s="44"/>
-      <c r="AF19" s="44"/>
-      <c r="AG19" s="43"/>
-      <c r="AH19" s="43"/>
-      <c r="AI19" s="43"/>
-      <c r="AJ19" s="43"/>
+      <c r="C19" s="47"/>
+      <c r="S19" s="42"/>
+      <c r="AG19" s="42"/>
+      <c r="AH19" s="42"/>
+      <c r="AI19" s="42"/>
+      <c r="AJ19" s="42"/>
       <c r="AK19" s="19"/>
-      <c r="AL19" s="43"/>
+      <c r="AL19" s="42"/>
       <c r="AM19" s="40"/>
       <c r="AN19" s="39"/>
-      <c r="AO19" s="43"/>
-      <c r="AP19" s="43"/>
-      <c r="AQ19" s="43"/>
-      <c r="AR19" s="47"/>
-      <c r="AS19" s="47"/>
-      <c r="AT19" s="47"/>
-      <c r="AU19" s="47"/>
-      <c r="AV19" s="47"/>
-      <c r="AW19" s="47"/>
-      <c r="AX19" s="47"/>
+      <c r="AO19" s="42"/>
+      <c r="AP19" s="42"/>
+      <c r="AQ19" s="42"/>
+      <c r="AR19" s="44"/>
+      <c r="AS19" s="44"/>
+      <c r="AT19" s="44"/>
+      <c r="AU19" s="44"/>
+      <c r="AV19" s="44"/>
+      <c r="AW19" s="44"/>
+      <c r="AX19" s="44"/>
     </row>
     <row r="20" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="32"/>
       <c r="B20" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="AE20" s="44"/>
-      <c r="AF20" s="44"/>
-      <c r="AG20" s="43"/>
-      <c r="AH20" s="43"/>
+      <c r="C20" s="47"/>
+      <c r="AG20" s="42"/>
+      <c r="AH20" s="42"/>
       <c r="AI20" s="19"/>
       <c r="AJ20" s="39"/>
-      <c r="AK20" s="43"/>
+      <c r="AK20" s="42"/>
       <c r="AL20" s="39"/>
-      <c r="AM20" s="43"/>
-      <c r="AN20" s="43"/>
-      <c r="AO20" s="43"/>
-      <c r="AP20" s="43"/>
-      <c r="AQ20" s="43"/>
-      <c r="AR20" s="43"/>
-      <c r="AS20" s="47"/>
-      <c r="AT20" s="47"/>
-      <c r="AU20" s="47"/>
-      <c r="AV20" s="47"/>
-      <c r="AW20" s="47"/>
-      <c r="AX20" s="47"/>
+      <c r="AM20" s="42"/>
+      <c r="AN20" s="42"/>
+      <c r="AO20" s="42"/>
+      <c r="AP20" s="42"/>
+      <c r="AQ20" s="42"/>
+      <c r="AR20" s="42"/>
+      <c r="AS20" s="44"/>
+      <c r="AT20" s="44"/>
+      <c r="AU20" s="44"/>
+      <c r="AV20" s="44"/>
+      <c r="AW20" s="44"/>
+      <c r="AX20" s="44"/>
     </row>
     <row r="21" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="32"/>
       <c r="B21" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="50"/>
-      <c r="AE21" s="44"/>
-      <c r="AF21" s="44"/>
-      <c r="AG21" s="44"/>
-      <c r="AH21" s="43"/>
+      <c r="C21" s="47"/>
+      <c r="AH21" s="42"/>
       <c r="AI21" s="19"/>
       <c r="AJ21" s="39"/>
-      <c r="AK21" s="43"/>
+      <c r="AK21" s="42"/>
       <c r="AL21" s="39"/>
-      <c r="AM21" s="44"/>
-      <c r="AN21" s="43"/>
-      <c r="AO21" s="43"/>
-      <c r="AP21" s="43"/>
-      <c r="AQ21" s="43"/>
-      <c r="AR21" s="47"/>
-      <c r="AS21" s="47"/>
-      <c r="AT21" s="47"/>
-      <c r="AU21" s="47"/>
-      <c r="AV21" s="47"/>
-      <c r="AW21" s="47"/>
-      <c r="AX21" s="47"/>
+      <c r="AN21" s="42"/>
+      <c r="AO21" s="42"/>
+      <c r="AP21" s="42"/>
+      <c r="AQ21" s="42"/>
+      <c r="AR21" s="44"/>
+      <c r="AS21" s="44"/>
+      <c r="AT21" s="44"/>
+      <c r="AU21" s="44"/>
+      <c r="AV21" s="44"/>
+      <c r="AW21" s="44"/>
+      <c r="AX21" s="44"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="32"/>
-      <c r="AE22" s="44"/>
-      <c r="AF22" s="44"/>
-      <c r="AG22" s="44"/>
-      <c r="AH22" s="44"/>
-      <c r="AI22" s="44"/>
-      <c r="AJ22" s="44"/>
-      <c r="AK22" s="44"/>
-      <c r="AL22" s="44"/>
-      <c r="AM22" s="44"/>
-      <c r="AN22" s="44"/>
-      <c r="AO22" s="44"/>
-      <c r="AP22" s="44"/>
-      <c r="AQ22" s="44"/>
-      <c r="AR22" s="44"/>
-      <c r="AS22" s="44"/>
-      <c r="AT22" s="44"/>
-      <c r="AU22" s="44"/>
-      <c r="AV22" s="44"/>
-      <c r="AW22" s="44"/>
-      <c r="AX22" s="44"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="32"/>
       <c r="B23" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="45"/>
-      <c r="O23" s="45"/>
-      <c r="P23" s="45"/>
-      <c r="Q23" s="45"/>
-      <c r="R23" s="45"/>
-      <c r="S23" s="45"/>
-      <c r="T23" s="45"/>
-      <c r="U23" s="45"/>
-      <c r="V23" s="45"/>
-      <c r="W23" s="45"/>
-      <c r="X23" s="45"/>
-      <c r="Y23" s="45"/>
-      <c r="Z23" s="45"/>
-      <c r="AA23" s="45"/>
-      <c r="AB23" s="45"/>
-      <c r="AC23" s="45"/>
-      <c r="AD23" s="45"/>
-      <c r="AE23" s="45"/>
-      <c r="AF23" s="45"/>
-      <c r="AG23" s="45"/>
-      <c r="AH23" s="45"/>
-      <c r="AI23" s="45"/>
-      <c r="AJ23" s="45"/>
-      <c r="AK23" s="45"/>
-      <c r="AL23" s="45"/>
-      <c r="AM23" s="45"/>
-      <c r="AN23" s="45"/>
-      <c r="AO23" s="45"/>
-      <c r="AP23" s="45"/>
-      <c r="AQ23" s="45"/>
-      <c r="AR23" s="45"/>
-      <c r="AS23" s="45"/>
-      <c r="AT23" s="45"/>
-      <c r="AU23" s="45"/>
-      <c r="AV23" s="45"/>
-      <c r="AW23" s="45"/>
-      <c r="AX23" s="45"/>
-      <c r="AY23" s="45"/>
-      <c r="AZ23" s="45"/>
-      <c r="BA23" s="45"/>
-      <c r="BB23" s="45"/>
-      <c r="BC23" s="45"/>
-      <c r="BD23" s="45"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="43"/>
+      <c r="S23" s="43"/>
+      <c r="T23" s="43"/>
+      <c r="U23" s="43"/>
+      <c r="V23" s="43"/>
+      <c r="W23" s="43"/>
+      <c r="X23" s="43"/>
+      <c r="Y23" s="43"/>
+      <c r="Z23" s="43"/>
+      <c r="AA23" s="43"/>
+      <c r="AB23" s="43"/>
+      <c r="AC23" s="43"/>
+      <c r="AD23" s="43"/>
+      <c r="AE23" s="43"/>
+      <c r="AF23" s="43"/>
+      <c r="AG23" s="43"/>
+      <c r="AH23" s="43"/>
+      <c r="AI23" s="43"/>
+      <c r="AJ23" s="43"/>
+      <c r="AK23" s="43"/>
+      <c r="AL23" s="43"/>
+      <c r="AM23" s="43"/>
+      <c r="AN23" s="43"/>
+      <c r="AO23" s="43"/>
+      <c r="AP23" s="43"/>
+      <c r="AQ23" s="43"/>
+      <c r="AR23" s="43"/>
+      <c r="AS23" s="43"/>
+      <c r="AT23" s="43"/>
+      <c r="AU23" s="43"/>
+      <c r="AV23" s="43"/>
+      <c r="AW23" s="43"/>
+      <c r="AX23" s="43"/>
+      <c r="AY23" s="43"/>
+      <c r="AZ23" s="43"/>
+      <c r="BA23" s="43"/>
+      <c r="BB23" s="43"/>
+      <c r="BC23" s="43"/>
+      <c r="BD23" s="43"/>
     </row>
     <row r="24" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="32"/>
       <c r="B24" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="52"/>
-      <c r="P24" s="52"/>
-      <c r="Q24" s="52"/>
-      <c r="R24" s="52"/>
-      <c r="S24" s="52"/>
-      <c r="T24" s="52"/>
-      <c r="U24" s="52"/>
-      <c r="V24" s="52"/>
-      <c r="W24" s="52"/>
-      <c r="X24" s="52"/>
-      <c r="Y24" s="52"/>
-      <c r="Z24" s="52"/>
-      <c r="AA24" s="52"/>
-      <c r="AB24" s="52"/>
-      <c r="AC24" s="52"/>
-      <c r="AD24" s="52"/>
-      <c r="AE24" s="52"/>
-      <c r="AF24" s="53"/>
-      <c r="AG24" s="53"/>
-      <c r="AH24" s="53"/>
-      <c r="AI24" s="54"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="49"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="49"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="49"/>
+      <c r="T24" s="49"/>
+      <c r="U24" s="49"/>
+      <c r="V24" s="49"/>
+      <c r="W24" s="49"/>
+      <c r="X24" s="49"/>
+      <c r="Y24" s="49"/>
+      <c r="Z24" s="49"/>
+      <c r="AA24" s="49"/>
+      <c r="AB24" s="49"/>
+      <c r="AC24" s="49"/>
+      <c r="AD24" s="49"/>
+      <c r="AE24" s="49"/>
+      <c r="AF24" s="49"/>
+      <c r="AG24" s="49"/>
+      <c r="AH24" s="49"/>
+      <c r="AI24" s="50"/>
       <c r="AJ24" s="40"/>
-      <c r="AK24" s="53"/>
+      <c r="AK24" s="49"/>
       <c r="AL24" s="40"/>
-      <c r="AM24" s="55"/>
-      <c r="AN24" s="53"/>
-      <c r="AO24" s="53"/>
-      <c r="AP24" s="53"/>
-      <c r="AQ24" s="53"/>
-      <c r="AR24" s="53"/>
-      <c r="AS24" s="53"/>
-      <c r="AT24" s="53"/>
-      <c r="AU24" s="52"/>
-      <c r="AV24" s="52"/>
-      <c r="AW24" s="52"/>
-      <c r="AX24" s="52"/>
-      <c r="AY24" s="52"/>
-      <c r="AZ24" s="52"/>
-      <c r="BA24" s="52"/>
-      <c r="BB24" s="52"/>
-      <c r="BC24" s="52"/>
-      <c r="BD24" s="52"/>
+      <c r="AM24" s="51"/>
+      <c r="AN24" s="49"/>
+      <c r="AO24" s="49"/>
+      <c r="AP24" s="49"/>
+      <c r="AQ24" s="49"/>
+      <c r="AR24" s="49"/>
+      <c r="AS24" s="49"/>
+      <c r="AT24" s="49"/>
+      <c r="AU24" s="49"/>
+      <c r="AV24" s="49"/>
+      <c r="AW24" s="49"/>
+      <c r="AX24" s="49"/>
+      <c r="AY24" s="49"/>
+      <c r="AZ24" s="49"/>
+      <c r="BA24" s="49"/>
+      <c r="BB24" s="49"/>
+      <c r="BC24" s="49"/>
+      <c r="BD24" s="49"/>
     </row>
     <row r="25" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="32"/>
       <c r="B25" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="56"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="57"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="57"/>
-      <c r="O25" s="57"/>
-      <c r="P25" s="57"/>
-      <c r="Q25" s="57"/>
-      <c r="R25" s="57"/>
-      <c r="S25" s="57"/>
-      <c r="T25" s="57"/>
-      <c r="U25" s="46"/>
-      <c r="V25" s="46"/>
-      <c r="W25" s="57"/>
-      <c r="X25" s="57"/>
-      <c r="Y25" s="57"/>
-      <c r="Z25" s="57"/>
-      <c r="AA25" s="57"/>
-      <c r="AB25" s="57"/>
-      <c r="AC25" s="57"/>
-      <c r="AD25" s="57"/>
-      <c r="AE25" s="57"/>
-      <c r="AF25" s="44"/>
-      <c r="AG25" s="44"/>
-      <c r="AH25" s="44"/>
-      <c r="AI25" s="44"/>
-      <c r="AJ25" s="44"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="53"/>
+      <c r="O25" s="53"/>
+      <c r="P25" s="53"/>
+      <c r="Q25" s="53"/>
+      <c r="R25" s="53"/>
+      <c r="S25" s="53"/>
+      <c r="T25" s="53"/>
+      <c r="U25" s="40"/>
+      <c r="V25" s="40"/>
+      <c r="W25" s="53"/>
+      <c r="X25" s="53"/>
+      <c r="Y25" s="53"/>
+      <c r="Z25" s="53"/>
+      <c r="AA25" s="53"/>
+      <c r="AB25" s="53"/>
+      <c r="AC25" s="53"/>
+      <c r="AD25" s="53"/>
+      <c r="AE25" s="53"/>
       <c r="AK25" s="40"/>
-      <c r="AL25" s="44"/>
-      <c r="AM25" s="47"/>
-      <c r="AN25" s="44"/>
-      <c r="AO25" s="44"/>
-      <c r="AP25" s="44"/>
-      <c r="AQ25" s="44"/>
-      <c r="AR25" s="47"/>
-      <c r="AS25" s="47"/>
-      <c r="AT25" s="44"/>
+      <c r="AM25" s="44"/>
+      <c r="AR25" s="44"/>
+      <c r="AS25" s="44"/>
     </row>
     <row r="26" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="32"/>
       <c r="B26" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="42"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
       <c r="F26" s="20"/>
-      <c r="V26" s="46"/>
-      <c r="AF26" s="44"/>
-      <c r="AG26" s="44"/>
-      <c r="AH26" s="44"/>
-      <c r="AI26" s="44"/>
-      <c r="AJ26" s="44"/>
-      <c r="AK26" s="44"/>
-      <c r="AL26" s="44"/>
-      <c r="AM26" s="43"/>
+      <c r="V26" s="40"/>
+      <c r="AM26" s="42"/>
       <c r="AN26" s="39"/>
       <c r="AO26" s="39"/>
-      <c r="AP26" s="43"/>
-      <c r="AQ26" s="43"/>
-      <c r="AR26" s="47"/>
-      <c r="AS26" s="47"/>
-      <c r="AT26" s="44"/>
+      <c r="AP26" s="42"/>
+      <c r="AQ26" s="42"/>
+      <c r="AR26" s="44"/>
+      <c r="AS26" s="44"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="32"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
       <c r="F27" s="20"/>
-      <c r="AF27" s="44"/>
-      <c r="AG27" s="44"/>
-      <c r="AH27" s="44"/>
-      <c r="AI27" s="44"/>
-      <c r="AJ27" s="44"/>
-      <c r="AK27" s="44"/>
-      <c r="AL27" s="44"/>
-      <c r="AM27" s="44"/>
-      <c r="AN27" s="44"/>
-      <c r="AO27" s="44"/>
-      <c r="AP27" s="44"/>
-      <c r="AQ27" s="44"/>
-      <c r="AR27" s="44"/>
-      <c r="AS27" s="44"/>
-      <c r="AT27" s="44"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="32"/>
       <c r="B28" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
       <c r="H28" s="25"/>
       <c r="I28" s="25"/>
     </row>
@@ -2315,92 +2211,72 @@
       <c r="B29" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="60"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="63"/>
-      <c r="J29" s="61"/>
-      <c r="K29" s="61"/>
-      <c r="L29" s="61"/>
-      <c r="M29" s="61"/>
-      <c r="N29" s="61"/>
-      <c r="O29" s="61"/>
-      <c r="P29" s="61"/>
-      <c r="Q29" s="61"/>
-      <c r="R29" s="61"/>
-      <c r="S29" s="61"/>
-      <c r="T29" s="61"/>
-      <c r="U29" s="61"/>
-      <c r="V29" s="61"/>
-      <c r="W29" s="61"/>
-      <c r="X29" s="61"/>
-      <c r="Y29" s="61"/>
-      <c r="Z29" s="61"/>
-      <c r="AA29" s="61"/>
-      <c r="AB29" s="61"/>
-      <c r="AC29" s="61"/>
-      <c r="AD29" s="61"/>
-      <c r="AE29" s="61"/>
-      <c r="AF29" s="61"/>
-      <c r="AG29" s="61"/>
-      <c r="AH29" s="61"/>
-      <c r="AI29" s="61"/>
-      <c r="AJ29" s="61"/>
-      <c r="AK29" s="61"/>
-      <c r="AL29" s="61"/>
-      <c r="AM29" s="64"/>
-      <c r="AN29" s="64"/>
-      <c r="AO29" s="65"/>
-      <c r="AP29" s="64"/>
-      <c r="AQ29" s="66"/>
-      <c r="AR29" s="64"/>
-      <c r="AS29" s="64"/>
-      <c r="AT29" s="67"/>
-      <c r="AU29" s="68"/>
-      <c r="AV29" s="68"/>
-      <c r="AW29" s="68"/>
-      <c r="AX29" s="68"/>
-      <c r="AY29" s="61"/>
-      <c r="AZ29" s="61"/>
-      <c r="BA29" s="61"/>
-      <c r="BB29" s="61"/>
-      <c r="BC29" s="61"/>
-      <c r="BD29" s="61"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="57"/>
+      <c r="L29" s="57"/>
+      <c r="M29" s="57"/>
+      <c r="N29" s="57"/>
+      <c r="O29" s="57"/>
+      <c r="P29" s="57"/>
+      <c r="Q29" s="57"/>
+      <c r="R29" s="57"/>
+      <c r="S29" s="57"/>
+      <c r="T29" s="57"/>
+      <c r="U29" s="57"/>
+      <c r="V29" s="57"/>
+      <c r="W29" s="57"/>
+      <c r="X29" s="57"/>
+      <c r="Y29" s="57"/>
+      <c r="Z29" s="57"/>
+      <c r="AA29" s="57"/>
+      <c r="AB29" s="57"/>
+      <c r="AC29" s="57"/>
+      <c r="AD29" s="57"/>
+      <c r="AE29" s="57"/>
+      <c r="AF29" s="57"/>
+      <c r="AG29" s="57"/>
+      <c r="AH29" s="57"/>
+      <c r="AI29" s="57"/>
+      <c r="AJ29" s="57"/>
+      <c r="AK29" s="57"/>
+      <c r="AL29" s="57"/>
+      <c r="AM29" s="57"/>
+      <c r="AN29" s="57"/>
+      <c r="AO29" s="60"/>
+      <c r="AP29" s="57"/>
+      <c r="AQ29" s="61"/>
+      <c r="AR29" s="57"/>
+      <c r="AS29" s="57"/>
+      <c r="AT29" s="62"/>
+      <c r="AU29" s="63"/>
+      <c r="AV29" s="63"/>
+      <c r="AW29" s="63"/>
+      <c r="AX29" s="63"/>
+      <c r="AY29" s="57"/>
+      <c r="AZ29" s="57"/>
+      <c r="BA29" s="57"/>
+      <c r="BB29" s="57"/>
+      <c r="BC29" s="57"/>
+      <c r="BD29" s="57"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="32"/>
       <c r="B30" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="AM30" s="44"/>
-      <c r="AN30" s="44"/>
-      <c r="AO30" s="44"/>
-      <c r="AP30" s="44"/>
-      <c r="AQ30" s="44"/>
-      <c r="AR30" s="49"/>
-      <c r="AS30" s="44"/>
-      <c r="AT30" s="43"/>
-      <c r="AU30" s="47"/>
+      <c r="AR30" s="46"/>
+      <c r="AT30" s="42"/>
+      <c r="AU30" s="44"/>
       <c r="AV30" s="14"/>
-      <c r="AW30" s="47"/>
-      <c r="AX30" s="47"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AM31" s="44"/>
-      <c r="AN31" s="44"/>
-      <c r="AO31" s="44"/>
-      <c r="AP31" s="44"/>
-      <c r="AQ31" s="44"/>
-      <c r="AR31" s="44"/>
-      <c r="AS31" s="44"/>
-      <c r="AT31" s="44"/>
-      <c r="AU31" s="44"/>
-      <c r="AV31" s="44"/>
-      <c r="AW31" s="44"/>
-      <c r="AX31" s="44"/>
+      <c r="AW30" s="44"/>
+      <c r="AX30" s="44"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="32" t="s">
@@ -2409,7 +2285,7 @@
       <c r="B32" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="69"/>
+      <c r="C32" s="64"/>
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
       <c r="F32" s="25"/>
@@ -2441,25 +2317,13 @@
       <c r="AF32" s="25"/>
       <c r="AG32" s="25"/>
       <c r="AH32" s="25"/>
-      <c r="AM32" s="44"/>
-      <c r="AN32" s="44"/>
-      <c r="AO32" s="44"/>
-      <c r="AP32" s="44"/>
-      <c r="AQ32" s="44"/>
-      <c r="AR32" s="44"/>
-      <c r="AS32" s="44"/>
-      <c r="AT32" s="44"/>
-      <c r="AU32" s="44"/>
-      <c r="AV32" s="44"/>
-      <c r="AW32" s="44"/>
-      <c r="AX32" s="44"/>
     </row>
     <row r="33" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="32"/>
       <c r="B33" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="70"/>
+      <c r="C33" s="65"/>
       <c r="D33" s="36"/>
       <c r="E33" s="36"/>
       <c r="F33" s="36"/>
@@ -2488,497 +2352,448 @@
       <c r="AC33" s="36"/>
       <c r="AD33" s="36"/>
       <c r="AE33" s="36"/>
-      <c r="AF33" s="71"/>
-      <c r="AG33" s="71"/>
-      <c r="AH33" s="71"/>
-      <c r="AI33" s="64"/>
-      <c r="AJ33" s="64"/>
-      <c r="AK33" s="65"/>
-      <c r="AL33" s="64"/>
-      <c r="AM33" s="64"/>
-      <c r="AN33" s="64"/>
-      <c r="AO33" s="64"/>
-      <c r="AP33" s="64"/>
-      <c r="AQ33" s="65"/>
-      <c r="AR33" s="65"/>
-      <c r="AS33" s="65"/>
-      <c r="AT33" s="65"/>
-      <c r="AU33" s="65"/>
-      <c r="AV33" s="67"/>
-      <c r="AW33" s="72"/>
-      <c r="AX33" s="67"/>
-      <c r="AY33" s="68"/>
-      <c r="AZ33" s="61"/>
-      <c r="BA33" s="61"/>
-      <c r="BB33" s="61"/>
-      <c r="BC33" s="61"/>
-      <c r="BD33" s="61"/>
+      <c r="AF33" s="66"/>
+      <c r="AG33" s="66"/>
+      <c r="AH33" s="66"/>
+      <c r="AI33" s="57"/>
+      <c r="AJ33" s="57"/>
+      <c r="AK33" s="60"/>
+      <c r="AL33" s="57"/>
+      <c r="AM33" s="57"/>
+      <c r="AN33" s="57"/>
+      <c r="AO33" s="57"/>
+      <c r="AP33" s="57"/>
+      <c r="AQ33" s="60"/>
+      <c r="AR33" s="60"/>
+      <c r="AS33" s="60"/>
+      <c r="AT33" s="60"/>
+      <c r="AU33" s="60"/>
+      <c r="AV33" s="62"/>
+      <c r="AW33" s="67"/>
+      <c r="AX33" s="62"/>
+      <c r="AY33" s="63"/>
+      <c r="AZ33" s="63"/>
+      <c r="BA33" s="57"/>
+      <c r="BB33" s="57"/>
+      <c r="BC33" s="57"/>
+      <c r="BD33" s="57"/>
     </row>
     <row r="34" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="32"/>
-      <c r="B34" s="57" t="s">
+      <c r="B34" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="56"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="57"/>
-      <c r="J34" s="57"/>
-      <c r="K34" s="57"/>
-      <c r="L34" s="57"/>
-      <c r="M34" s="57"/>
-      <c r="N34" s="57"/>
-      <c r="O34" s="57"/>
-      <c r="P34" s="57"/>
-      <c r="Q34" s="57"/>
-      <c r="R34" s="57"/>
-      <c r="S34" s="57"/>
-      <c r="T34" s="57"/>
-      <c r="U34" s="57"/>
-      <c r="V34" s="57"/>
-      <c r="W34" s="57"/>
-      <c r="X34" s="57"/>
-      <c r="Y34" s="57"/>
-      <c r="Z34" s="57"/>
-      <c r="AA34" s="57"/>
-      <c r="AB34" s="57"/>
-      <c r="AC34" s="57"/>
-      <c r="AD34" s="57"/>
-      <c r="AE34" s="57"/>
-      <c r="AF34" s="73"/>
-      <c r="AG34" s="73"/>
-      <c r="AH34" s="73"/>
-      <c r="AI34" s="44"/>
-      <c r="AJ34" s="44"/>
-      <c r="AK34" s="49"/>
-      <c r="AL34" s="44"/>
-      <c r="AM34" s="44"/>
-      <c r="AN34" s="44"/>
-      <c r="AO34" s="44"/>
-      <c r="AP34" s="44"/>
-      <c r="AQ34" s="49"/>
-      <c r="AR34" s="49"/>
-      <c r="AS34" s="49"/>
-      <c r="AT34" s="49"/>
-      <c r="AU34" s="49"/>
-      <c r="AV34" s="44"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="53"/>
+      <c r="L34" s="53"/>
+      <c r="M34" s="53"/>
+      <c r="N34" s="53"/>
+      <c r="O34" s="53"/>
+      <c r="P34" s="53"/>
+      <c r="Q34" s="53"/>
+      <c r="R34" s="53"/>
+      <c r="S34" s="53"/>
+      <c r="T34" s="53"/>
+      <c r="U34" s="53"/>
+      <c r="V34" s="53"/>
+      <c r="W34" s="53"/>
+      <c r="X34" s="53"/>
+      <c r="Y34" s="53"/>
+      <c r="Z34" s="53"/>
+      <c r="AA34" s="53"/>
+      <c r="AB34" s="53"/>
+      <c r="AC34" s="53"/>
+      <c r="AD34" s="53"/>
+      <c r="AE34" s="53"/>
+      <c r="AF34" s="68"/>
+      <c r="AG34" s="68"/>
+      <c r="AH34" s="68"/>
+      <c r="AK34" s="46"/>
+      <c r="AQ34" s="46"/>
+      <c r="AR34" s="46"/>
+      <c r="AS34" s="46"/>
+      <c r="AT34" s="46"/>
+      <c r="AU34" s="46"/>
       <c r="AW34" s="39"/>
-      <c r="AX34" s="43"/>
-      <c r="AY34" s="47"/>
+      <c r="AX34" s="42"/>
+      <c r="AY34" s="44"/>
+      <c r="AZ34" s="44"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="32"/>
       <c r="B35" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="69"/>
-      <c r="D35" s="73"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="73"/>
-      <c r="G35" s="73"/>
-      <c r="H35" s="73"/>
-      <c r="I35" s="73"/>
-      <c r="J35" s="73"/>
-      <c r="K35" s="73"/>
-      <c r="L35" s="73"/>
-      <c r="M35" s="73"/>
-      <c r="N35" s="73"/>
-      <c r="O35" s="73"/>
-      <c r="P35" s="73"/>
-      <c r="Q35" s="73"/>
-      <c r="R35" s="73"/>
-      <c r="S35" s="73"/>
-      <c r="T35" s="73"/>
-      <c r="U35" s="73"/>
-      <c r="V35" s="73"/>
-      <c r="W35" s="73"/>
-      <c r="X35" s="73"/>
-      <c r="Y35" s="73"/>
-      <c r="Z35" s="73"/>
-      <c r="AA35" s="73"/>
-      <c r="AB35" s="73"/>
-      <c r="AC35" s="73"/>
-      <c r="AD35" s="73"/>
-      <c r="AE35" s="73"/>
-      <c r="AF35" s="73"/>
-      <c r="AG35" s="73"/>
-      <c r="AH35" s="73"/>
-      <c r="AI35" s="44"/>
-      <c r="AJ35" s="44"/>
-      <c r="AK35" s="49"/>
-      <c r="AL35" s="44"/>
-      <c r="AM35" s="44"/>
-      <c r="AN35" s="44"/>
-      <c r="AO35" s="44"/>
-      <c r="AP35" s="44"/>
-      <c r="AQ35" s="49"/>
-      <c r="AR35" s="49"/>
-      <c r="AS35" s="49"/>
-      <c r="AT35" s="49"/>
-      <c r="AU35" s="49"/>
-      <c r="AV35" s="44"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="68"/>
+      <c r="J35" s="68"/>
+      <c r="K35" s="68"/>
+      <c r="L35" s="68"/>
+      <c r="M35" s="68"/>
+      <c r="N35" s="68"/>
+      <c r="O35" s="68"/>
+      <c r="P35" s="68"/>
+      <c r="Q35" s="68"/>
+      <c r="R35" s="68"/>
+      <c r="S35" s="68"/>
+      <c r="T35" s="68"/>
+      <c r="U35" s="68"/>
+      <c r="V35" s="68"/>
+      <c r="W35" s="68"/>
+      <c r="X35" s="68"/>
+      <c r="Y35" s="68"/>
+      <c r="Z35" s="68"/>
+      <c r="AA35" s="68"/>
+      <c r="AB35" s="68"/>
+      <c r="AC35" s="68"/>
+      <c r="AD35" s="68"/>
+      <c r="AE35" s="68"/>
+      <c r="AF35" s="68"/>
+      <c r="AG35" s="68"/>
+      <c r="AH35" s="68"/>
+      <c r="AK35" s="46"/>
+      <c r="AQ35" s="46"/>
+      <c r="AR35" s="46"/>
+      <c r="AS35" s="46"/>
+      <c r="AT35" s="46"/>
+      <c r="AU35" s="46"/>
       <c r="AW35" s="39"/>
-      <c r="AX35" s="43"/>
-      <c r="AY35" s="47"/>
+      <c r="AX35" s="42"/>
+      <c r="AY35" s="44"/>
+      <c r="AZ35" s="44"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="32"/>
       <c r="B36" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="69"/>
+      <c r="C36" s="64"/>
       <c r="D36" s="25"/>
       <c r="E36" s="25"/>
       <c r="F36" s="25"/>
       <c r="G36" s="25"/>
       <c r="H36" s="25"/>
       <c r="I36" s="25"/>
-      <c r="J36" s="73"/>
-      <c r="K36" s="73"/>
-      <c r="L36" s="73"/>
-      <c r="M36" s="73"/>
-      <c r="N36" s="73"/>
-      <c r="O36" s="73"/>
-      <c r="P36" s="73"/>
-      <c r="Q36" s="73"/>
-      <c r="R36" s="73"/>
-      <c r="S36" s="73"/>
-      <c r="T36" s="73"/>
-      <c r="U36" s="73"/>
-      <c r="V36" s="73"/>
-      <c r="W36" s="73"/>
-      <c r="X36" s="73"/>
-      <c r="Y36" s="73"/>
-      <c r="Z36" s="73"/>
-      <c r="AA36" s="73"/>
-      <c r="AB36" s="73"/>
-      <c r="AC36" s="73"/>
-      <c r="AD36" s="73"/>
-      <c r="AE36" s="73"/>
-      <c r="AF36" s="73"/>
-      <c r="AG36" s="73"/>
-      <c r="AH36" s="73"/>
-      <c r="AI36" s="44"/>
-      <c r="AJ36" s="44"/>
-      <c r="AK36" s="49"/>
-      <c r="AL36" s="44"/>
-      <c r="AM36" s="44"/>
-      <c r="AN36" s="44"/>
-      <c r="AO36" s="44"/>
-      <c r="AP36" s="44"/>
-      <c r="AQ36" s="49"/>
-      <c r="AR36" s="49"/>
-      <c r="AS36" s="49"/>
-      <c r="AT36" s="49"/>
-      <c r="AU36" s="49"/>
-      <c r="AV36" s="44"/>
+      <c r="J36" s="68"/>
+      <c r="K36" s="68"/>
+      <c r="L36" s="68"/>
+      <c r="M36" s="68"/>
+      <c r="N36" s="68"/>
+      <c r="O36" s="68"/>
+      <c r="P36" s="68"/>
+      <c r="Q36" s="68"/>
+      <c r="R36" s="68"/>
+      <c r="S36" s="68"/>
+      <c r="T36" s="68"/>
+      <c r="U36" s="68"/>
+      <c r="V36" s="68"/>
+      <c r="W36" s="68"/>
+      <c r="X36" s="68"/>
+      <c r="Y36" s="68"/>
+      <c r="Z36" s="68"/>
+      <c r="AA36" s="68"/>
+      <c r="AB36" s="68"/>
+      <c r="AC36" s="68"/>
+      <c r="AD36" s="68"/>
+      <c r="AE36" s="68"/>
+      <c r="AF36" s="68"/>
+      <c r="AG36" s="68"/>
+      <c r="AH36" s="68"/>
+      <c r="AK36" s="46"/>
+      <c r="AQ36" s="46"/>
+      <c r="AR36" s="46"/>
+      <c r="AS36" s="46"/>
+      <c r="AT36" s="46"/>
+      <c r="AU36" s="46"/>
       <c r="AW36" s="39"/>
-      <c r="AX36" s="43"/>
-      <c r="AY36" s="47"/>
+      <c r="AX36" s="42"/>
+      <c r="AY36" s="44"/>
+      <c r="AZ36" s="44"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="32"/>
       <c r="B37" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="69"/>
+      <c r="C37" s="64"/>
       <c r="D37" s="25"/>
       <c r="E37" s="25"/>
       <c r="F37" s="25"/>
       <c r="G37" s="25"/>
       <c r="H37" s="25"/>
       <c r="I37" s="25"/>
-      <c r="J37" s="73"/>
-      <c r="K37" s="73"/>
-      <c r="L37" s="73"/>
-      <c r="M37" s="73"/>
-      <c r="N37" s="73"/>
-      <c r="O37" s="73"/>
-      <c r="P37" s="73"/>
-      <c r="Q37" s="73"/>
-      <c r="R37" s="73"/>
-      <c r="S37" s="73"/>
-      <c r="T37" s="73"/>
-      <c r="U37" s="73"/>
-      <c r="V37" s="73"/>
-      <c r="W37" s="73"/>
-      <c r="X37" s="73"/>
-      <c r="Y37" s="73"/>
-      <c r="Z37" s="73"/>
-      <c r="AA37" s="73"/>
-      <c r="AB37" s="73"/>
-      <c r="AC37" s="73"/>
-      <c r="AD37" s="73"/>
-      <c r="AE37" s="73"/>
-      <c r="AF37" s="73"/>
-      <c r="AG37" s="73"/>
-      <c r="AH37" s="73"/>
-      <c r="AI37" s="44"/>
-      <c r="AJ37" s="44"/>
-      <c r="AK37" s="49"/>
-      <c r="AL37" s="44"/>
-      <c r="AM37" s="44"/>
-      <c r="AN37" s="44"/>
-      <c r="AO37" s="44"/>
-      <c r="AP37" s="44"/>
-      <c r="AQ37" s="49"/>
-      <c r="AR37" s="49"/>
-      <c r="AS37" s="49"/>
-      <c r="AT37" s="49"/>
-      <c r="AU37" s="49"/>
-      <c r="AV37" s="44"/>
+      <c r="J37" s="68"/>
+      <c r="K37" s="68"/>
+      <c r="L37" s="68"/>
+      <c r="M37" s="68"/>
+      <c r="N37" s="68"/>
+      <c r="O37" s="68"/>
+      <c r="P37" s="68"/>
+      <c r="Q37" s="68"/>
+      <c r="R37" s="68"/>
+      <c r="S37" s="68"/>
+      <c r="T37" s="68"/>
+      <c r="U37" s="68"/>
+      <c r="V37" s="68"/>
+      <c r="W37" s="68"/>
+      <c r="X37" s="68"/>
+      <c r="Y37" s="68"/>
+      <c r="Z37" s="68"/>
+      <c r="AA37" s="68"/>
+      <c r="AB37" s="68"/>
+      <c r="AC37" s="68"/>
+      <c r="AD37" s="68"/>
+      <c r="AE37" s="68"/>
+      <c r="AF37" s="68"/>
+      <c r="AG37" s="68"/>
+      <c r="AH37" s="68"/>
+      <c r="AK37" s="46"/>
+      <c r="AQ37" s="46"/>
+      <c r="AR37" s="46"/>
+      <c r="AS37" s="46"/>
+      <c r="AT37" s="46"/>
+      <c r="AU37" s="46"/>
       <c r="AW37" s="40"/>
-      <c r="AX37" s="43"/>
-      <c r="AY37" s="47"/>
+      <c r="AX37" s="42"/>
+      <c r="AY37" s="44"/>
+      <c r="AZ37" s="44"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="32"/>
       <c r="B38" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="69"/>
+      <c r="C38" s="64"/>
       <c r="D38" s="25"/>
       <c r="E38" s="25"/>
       <c r="F38" s="25"/>
       <c r="G38" s="25"/>
       <c r="H38" s="25"/>
       <c r="I38" s="25"/>
-      <c r="J38" s="73"/>
-      <c r="K38" s="73"/>
-      <c r="L38" s="73"/>
-      <c r="M38" s="73"/>
-      <c r="N38" s="73"/>
-      <c r="O38" s="73"/>
-      <c r="P38" s="73"/>
-      <c r="Q38" s="73"/>
-      <c r="R38" s="73"/>
-      <c r="S38" s="73"/>
-      <c r="T38" s="73"/>
-      <c r="U38" s="73"/>
-      <c r="V38" s="73"/>
-      <c r="W38" s="73"/>
-      <c r="X38" s="73"/>
-      <c r="Y38" s="73"/>
-      <c r="Z38" s="73"/>
-      <c r="AA38" s="73"/>
-      <c r="AB38" s="73"/>
-      <c r="AC38" s="73"/>
-      <c r="AD38" s="73"/>
-      <c r="AE38" s="73"/>
-      <c r="AF38" s="73"/>
-      <c r="AG38" s="73"/>
-      <c r="AH38" s="73"/>
-      <c r="AI38" s="44"/>
-      <c r="AJ38" s="44"/>
-      <c r="AK38" s="49"/>
-      <c r="AL38" s="44"/>
-      <c r="AM38" s="44"/>
-      <c r="AN38" s="44"/>
-      <c r="AO38" s="44"/>
-      <c r="AP38" s="44"/>
-      <c r="AQ38" s="49"/>
-      <c r="AR38" s="49"/>
-      <c r="AS38" s="49"/>
-      <c r="AT38" s="49"/>
-      <c r="AU38" s="49"/>
-      <c r="AV38" s="44"/>
+      <c r="J38" s="68"/>
+      <c r="K38" s="68"/>
+      <c r="L38" s="68"/>
+      <c r="M38" s="68"/>
+      <c r="N38" s="68"/>
+      <c r="O38" s="68"/>
+      <c r="P38" s="68"/>
+      <c r="Q38" s="68"/>
+      <c r="R38" s="68"/>
+      <c r="S38" s="68"/>
+      <c r="T38" s="68"/>
+      <c r="U38" s="68"/>
+      <c r="V38" s="68"/>
+      <c r="W38" s="68"/>
+      <c r="X38" s="68"/>
+      <c r="Y38" s="68"/>
+      <c r="Z38" s="68"/>
+      <c r="AA38" s="68"/>
+      <c r="AB38" s="68"/>
+      <c r="AC38" s="68"/>
+      <c r="AD38" s="68"/>
+      <c r="AE38" s="68"/>
+      <c r="AF38" s="68"/>
+      <c r="AG38" s="68"/>
+      <c r="AH38" s="68"/>
+      <c r="AK38" s="46"/>
+      <c r="AQ38" s="46"/>
+      <c r="AR38" s="46"/>
+      <c r="AS38" s="46"/>
+      <c r="AT38" s="46"/>
+      <c r="AU38" s="46"/>
       <c r="AW38" s="40"/>
-      <c r="AX38" s="43"/>
-      <c r="AY38" s="47"/>
+      <c r="AX38" s="42"/>
+      <c r="AY38" s="44"/>
+      <c r="AZ38" s="44"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="32"/>
       <c r="B39" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="69"/>
+      <c r="C39" s="64"/>
       <c r="D39" s="25"/>
       <c r="E39" s="25"/>
       <c r="F39" s="25"/>
       <c r="G39" s="25"/>
       <c r="H39" s="25"/>
       <c r="I39" s="25"/>
-      <c r="J39" s="73"/>
-      <c r="K39" s="73"/>
-      <c r="L39" s="73"/>
-      <c r="M39" s="73"/>
-      <c r="N39" s="73"/>
-      <c r="O39" s="73"/>
-      <c r="P39" s="73"/>
-      <c r="Q39" s="73"/>
-      <c r="R39" s="73"/>
-      <c r="S39" s="73"/>
-      <c r="T39" s="73"/>
-      <c r="U39" s="73"/>
-      <c r="V39" s="73"/>
-      <c r="W39" s="73"/>
-      <c r="X39" s="73"/>
-      <c r="Y39" s="73"/>
-      <c r="Z39" s="73"/>
-      <c r="AA39" s="73"/>
-      <c r="AB39" s="73"/>
-      <c r="AC39" s="73"/>
-      <c r="AD39" s="73"/>
-      <c r="AE39" s="73"/>
-      <c r="AF39" s="73"/>
-      <c r="AG39" s="73"/>
-      <c r="AH39" s="73"/>
-      <c r="AI39" s="44"/>
-      <c r="AJ39" s="44"/>
-      <c r="AK39" s="49"/>
-      <c r="AL39" s="44"/>
-      <c r="AM39" s="44"/>
-      <c r="AN39" s="44"/>
-      <c r="AO39" s="44"/>
-      <c r="AP39" s="44"/>
-      <c r="AQ39" s="49"/>
-      <c r="AR39" s="49"/>
-      <c r="AS39" s="49"/>
-      <c r="AT39" s="49"/>
-      <c r="AU39" s="49"/>
-      <c r="AV39" s="44"/>
+      <c r="J39" s="68"/>
+      <c r="K39" s="68"/>
+      <c r="L39" s="68"/>
+      <c r="M39" s="68"/>
+      <c r="N39" s="68"/>
+      <c r="O39" s="68"/>
+      <c r="P39" s="68"/>
+      <c r="Q39" s="68"/>
+      <c r="R39" s="68"/>
+      <c r="S39" s="68"/>
+      <c r="T39" s="68"/>
+      <c r="U39" s="68"/>
+      <c r="V39" s="68"/>
+      <c r="W39" s="68"/>
+      <c r="X39" s="68"/>
+      <c r="Y39" s="68"/>
+      <c r="Z39" s="68"/>
+      <c r="AA39" s="68"/>
+      <c r="AB39" s="68"/>
+      <c r="AC39" s="68"/>
+      <c r="AD39" s="68"/>
+      <c r="AE39" s="68"/>
+      <c r="AF39" s="68"/>
+      <c r="AG39" s="68"/>
+      <c r="AH39" s="68"/>
+      <c r="AK39" s="46"/>
+      <c r="AQ39" s="46"/>
+      <c r="AR39" s="46"/>
+      <c r="AS39" s="46"/>
+      <c r="AT39" s="46"/>
+      <c r="AU39" s="46"/>
       <c r="AW39" s="40"/>
-      <c r="AX39" s="43"/>
-      <c r="AY39" s="47"/>
+      <c r="AX39" s="42"/>
+      <c r="AY39" s="44"/>
+      <c r="AZ39" s="44"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="32"/>
       <c r="B40" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="69"/>
+      <c r="C40" s="64"/>
       <c r="D40" s="25"/>
       <c r="E40" s="25"/>
       <c r="F40" s="25"/>
       <c r="G40" s="25"/>
       <c r="H40" s="25"/>
       <c r="I40" s="25"/>
-      <c r="J40" s="73"/>
-      <c r="K40" s="73"/>
-      <c r="L40" s="73"/>
-      <c r="M40" s="73"/>
-      <c r="N40" s="73"/>
-      <c r="O40" s="73"/>
-      <c r="P40" s="73"/>
-      <c r="Q40" s="73"/>
-      <c r="R40" s="73"/>
-      <c r="S40" s="73"/>
-      <c r="T40" s="73"/>
-      <c r="U40" s="73"/>
-      <c r="V40" s="73"/>
-      <c r="W40" s="73"/>
-      <c r="X40" s="73"/>
-      <c r="Y40" s="73"/>
-      <c r="Z40" s="73"/>
-      <c r="AA40" s="73"/>
-      <c r="AB40" s="73"/>
-      <c r="AC40" s="73"/>
-      <c r="AD40" s="73"/>
-      <c r="AE40" s="73"/>
-      <c r="AF40" s="73"/>
-      <c r="AG40" s="73"/>
-      <c r="AH40" s="73"/>
-      <c r="AI40" s="44"/>
-      <c r="AJ40" s="44"/>
-      <c r="AK40" s="49"/>
-      <c r="AL40" s="44"/>
-      <c r="AM40" s="44"/>
-      <c r="AN40" s="44"/>
-      <c r="AO40" s="44"/>
-      <c r="AP40" s="44"/>
-      <c r="AQ40" s="49"/>
-      <c r="AR40" s="49"/>
-      <c r="AS40" s="49"/>
-      <c r="AT40" s="49"/>
-      <c r="AU40" s="49"/>
-      <c r="AV40" s="44"/>
+      <c r="J40" s="68"/>
+      <c r="K40" s="68"/>
+      <c r="L40" s="68"/>
+      <c r="M40" s="68"/>
+      <c r="N40" s="68"/>
+      <c r="O40" s="68"/>
+      <c r="P40" s="68"/>
+      <c r="Q40" s="68"/>
+      <c r="R40" s="68"/>
+      <c r="S40" s="68"/>
+      <c r="T40" s="68"/>
+      <c r="U40" s="68"/>
+      <c r="V40" s="68"/>
+      <c r="W40" s="68"/>
+      <c r="X40" s="68"/>
+      <c r="Y40" s="68"/>
+      <c r="Z40" s="68"/>
+      <c r="AA40" s="68"/>
+      <c r="AB40" s="68"/>
+      <c r="AC40" s="68"/>
+      <c r="AD40" s="68"/>
+      <c r="AE40" s="68"/>
+      <c r="AF40" s="68"/>
+      <c r="AG40" s="68"/>
+      <c r="AH40" s="68"/>
+      <c r="AK40" s="46"/>
+      <c r="AQ40" s="46"/>
+      <c r="AR40" s="46"/>
+      <c r="AS40" s="46"/>
+      <c r="AT40" s="46"/>
+      <c r="AU40" s="46"/>
       <c r="AW40" s="40"/>
-      <c r="AX40" s="43"/>
-      <c r="AY40" s="47"/>
+      <c r="AX40" s="42"/>
+      <c r="AY40" s="44"/>
+      <c r="AZ40" s="44"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="32"/>
       <c r="B41" s="25"/>
-      <c r="C41" s="69"/>
-      <c r="D41" s="73"/>
-      <c r="E41" s="73"/>
-      <c r="F41" s="73"/>
-      <c r="G41" s="73"/>
-      <c r="H41" s="73"/>
-      <c r="I41" s="73"/>
-      <c r="J41" s="73"/>
-      <c r="K41" s="73"/>
-      <c r="L41" s="73"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="68"/>
+      <c r="H41" s="68"/>
+      <c r="I41" s="68"/>
+      <c r="J41" s="68"/>
+      <c r="K41" s="68"/>
+      <c r="L41" s="68"/>
       <c r="M41" s="25"/>
-      <c r="N41" s="73"/>
-      <c r="O41" s="73"/>
-      <c r="P41" s="73"/>
-      <c r="Q41" s="73"/>
-      <c r="R41" s="73"/>
-      <c r="S41" s="73"/>
-      <c r="T41" s="73"/>
-      <c r="U41" s="73"/>
-      <c r="V41" s="73"/>
-      <c r="W41" s="73"/>
-      <c r="X41" s="73"/>
-      <c r="Y41" s="73"/>
-      <c r="Z41" s="73"/>
-      <c r="AA41" s="73"/>
-      <c r="AB41" s="73"/>
-      <c r="AC41" s="73"/>
-      <c r="AD41" s="73"/>
-      <c r="AE41" s="73"/>
-      <c r="AF41" s="73"/>
-      <c r="AG41" s="73"/>
-      <c r="AH41" s="73"/>
+      <c r="N41" s="68"/>
+      <c r="O41" s="68"/>
+      <c r="P41" s="68"/>
+      <c r="Q41" s="68"/>
+      <c r="R41" s="68"/>
+      <c r="S41" s="68"/>
+      <c r="T41" s="68"/>
+      <c r="U41" s="68"/>
+      <c r="V41" s="68"/>
+      <c r="W41" s="68"/>
+      <c r="X41" s="68"/>
+      <c r="Y41" s="68"/>
+      <c r="Z41" s="68"/>
+      <c r="AA41" s="68"/>
+      <c r="AB41" s="68"/>
+      <c r="AC41" s="68"/>
+      <c r="AD41" s="68"/>
+      <c r="AE41" s="68"/>
+      <c r="AF41" s="68"/>
+      <c r="AG41" s="68"/>
+      <c r="AH41" s="68"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="32"/>
       <c r="B42" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="69"/>
-      <c r="D42" s="73"/>
-      <c r="E42" s="73"/>
-      <c r="F42" s="73"/>
-      <c r="G42" s="73"/>
-      <c r="H42" s="73"/>
-      <c r="I42" s="73"/>
-      <c r="J42" s="73"/>
-      <c r="K42" s="73"/>
-      <c r="L42" s="73"/>
-      <c r="M42" s="73"/>
-      <c r="N42" s="73"/>
-      <c r="O42" s="73"/>
-      <c r="P42" s="73"/>
-      <c r="Q42" s="73"/>
-      <c r="R42" s="73"/>
-      <c r="S42" s="73"/>
-      <c r="T42" s="73"/>
-      <c r="U42" s="73"/>
-      <c r="V42" s="73"/>
-      <c r="W42" s="73"/>
-      <c r="X42" s="73"/>
-      <c r="Y42" s="73"/>
-      <c r="Z42" s="73"/>
-      <c r="AA42" s="73"/>
-      <c r="AB42" s="73"/>
-      <c r="AC42" s="73"/>
-      <c r="AD42" s="73"/>
-      <c r="AE42" s="73"/>
-      <c r="AF42" s="73"/>
-      <c r="AG42" s="73"/>
-      <c r="AH42" s="73"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="68"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="68"/>
+      <c r="H42" s="68"/>
+      <c r="I42" s="68"/>
+      <c r="J42" s="68"/>
+      <c r="K42" s="68"/>
+      <c r="L42" s="68"/>
+      <c r="M42" s="68"/>
+      <c r="N42" s="68"/>
+      <c r="O42" s="68"/>
+      <c r="P42" s="68"/>
+      <c r="Q42" s="68"/>
+      <c r="R42" s="68"/>
+      <c r="S42" s="68"/>
+      <c r="T42" s="68"/>
+      <c r="U42" s="68"/>
+      <c r="V42" s="68"/>
+      <c r="W42" s="68"/>
+      <c r="X42" s="68"/>
+      <c r="Y42" s="68"/>
+      <c r="Z42" s="68"/>
+      <c r="AA42" s="68"/>
+      <c r="AB42" s="68"/>
+      <c r="AC42" s="68"/>
+      <c r="AD42" s="68"/>
+      <c r="AE42" s="68"/>
+      <c r="AF42" s="68"/>
+      <c r="AG42" s="68"/>
+      <c r="AH42" s="68"/>
     </row>
     <row r="43" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="32"/>
       <c r="B43" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="70"/>
+      <c r="C43" s="65"/>
       <c r="D43" s="36"/>
       <c r="E43" s="36"/>
       <c r="F43" s="36"/>
@@ -3007,199 +2822,187 @@
       <c r="AC43" s="36"/>
       <c r="AD43" s="36"/>
       <c r="AE43" s="36"/>
-      <c r="AF43" s="71"/>
-      <c r="AG43" s="71"/>
-      <c r="AH43" s="71"/>
-      <c r="AI43" s="61"/>
-      <c r="AJ43" s="61"/>
-      <c r="AK43" s="61"/>
-      <c r="AL43" s="61"/>
-      <c r="AM43" s="61"/>
-      <c r="AN43" s="61"/>
-      <c r="AO43" s="61"/>
-      <c r="AP43" s="61"/>
-      <c r="AQ43" s="61"/>
-      <c r="AR43" s="61"/>
-      <c r="AS43" s="61"/>
-      <c r="AT43" s="64"/>
-      <c r="AU43" s="64"/>
-      <c r="AV43" s="66"/>
-      <c r="AW43" s="64"/>
-      <c r="AX43" s="61"/>
-      <c r="AY43" s="61"/>
-      <c r="AZ43" s="61"/>
-      <c r="BA43" s="61"/>
-      <c r="BB43" s="61"/>
-      <c r="BC43" s="61"/>
-      <c r="BD43" s="61"/>
+      <c r="AF43" s="66"/>
+      <c r="AG43" s="66"/>
+      <c r="AH43" s="66"/>
+      <c r="AI43" s="57"/>
+      <c r="AJ43" s="57"/>
+      <c r="AK43" s="57"/>
+      <c r="AL43" s="57"/>
+      <c r="AM43" s="57"/>
+      <c r="AN43" s="57"/>
+      <c r="AO43" s="57"/>
+      <c r="AP43" s="57"/>
+      <c r="AQ43" s="57"/>
+      <c r="AR43" s="57"/>
+      <c r="AS43" s="57"/>
+      <c r="AT43" s="57"/>
+      <c r="AU43" s="57"/>
+      <c r="AV43" s="61"/>
+      <c r="AW43" s="57"/>
+      <c r="AX43" s="57"/>
+      <c r="AY43" s="57"/>
+      <c r="AZ43" s="57"/>
+      <c r="BA43" s="57"/>
+      <c r="BB43" s="57"/>
+      <c r="BC43" s="57"/>
+      <c r="BD43" s="57"/>
     </row>
     <row r="44" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="32"/>
-      <c r="B44" s="57" t="s">
+      <c r="B44" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="69"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="57"/>
-      <c r="H44" s="57"/>
-      <c r="I44" s="57"/>
-      <c r="J44" s="57"/>
-      <c r="K44" s="57"/>
-      <c r="L44" s="57"/>
-      <c r="M44" s="57"/>
-      <c r="N44" s="57"/>
-      <c r="O44" s="57"/>
-      <c r="P44" s="57"/>
-      <c r="Q44" s="57"/>
-      <c r="R44" s="57"/>
-      <c r="S44" s="57"/>
-      <c r="T44" s="57"/>
-      <c r="U44" s="57"/>
-      <c r="V44" s="57"/>
-      <c r="W44" s="57"/>
-      <c r="X44" s="57"/>
-      <c r="Y44" s="57"/>
-      <c r="Z44" s="57"/>
-      <c r="AA44" s="57"/>
-      <c r="AB44" s="57"/>
-      <c r="AC44" s="57"/>
-      <c r="AD44" s="57"/>
-      <c r="AE44" s="57"/>
-      <c r="AF44" s="73"/>
-      <c r="AG44" s="73"/>
-      <c r="AH44" s="73"/>
-      <c r="AT44" s="44"/>
-      <c r="AU44" s="44"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
+      <c r="K44" s="53"/>
+      <c r="L44" s="53"/>
+      <c r="M44" s="53"/>
+      <c r="N44" s="53"/>
+      <c r="O44" s="53"/>
+      <c r="P44" s="53"/>
+      <c r="Q44" s="53"/>
+      <c r="R44" s="53"/>
+      <c r="S44" s="53"/>
+      <c r="T44" s="53"/>
+      <c r="U44" s="53"/>
+      <c r="V44" s="53"/>
+      <c r="W44" s="53"/>
+      <c r="X44" s="53"/>
+      <c r="Y44" s="53"/>
+      <c r="Z44" s="53"/>
+      <c r="AA44" s="53"/>
+      <c r="AB44" s="53"/>
+      <c r="AC44" s="53"/>
+      <c r="AD44" s="53"/>
+      <c r="AE44" s="53"/>
+      <c r="AF44" s="68"/>
+      <c r="AG44" s="68"/>
+      <c r="AH44" s="68"/>
       <c r="AV44" s="40"/>
-      <c r="AW44" s="44"/>
     </row>
     <row r="45" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="32"/>
       <c r="B45" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="69"/>
-      <c r="D45" s="73"/>
-      <c r="E45" s="73"/>
-      <c r="F45" s="73"/>
-      <c r="G45" s="73"/>
-      <c r="H45" s="73"/>
-      <c r="I45" s="73"/>
-      <c r="J45" s="73"/>
-      <c r="K45" s="73"/>
-      <c r="L45" s="73"/>
-      <c r="M45" s="73"/>
-      <c r="N45" s="73"/>
-      <c r="O45" s="73"/>
-      <c r="P45" s="73"/>
-      <c r="Q45" s="73"/>
-      <c r="R45" s="73"/>
-      <c r="S45" s="73"/>
-      <c r="T45" s="73"/>
-      <c r="U45" s="73"/>
-      <c r="V45" s="73"/>
-      <c r="W45" s="73"/>
-      <c r="X45" s="73"/>
-      <c r="Y45" s="73"/>
-      <c r="Z45" s="73"/>
-      <c r="AA45" s="73"/>
-      <c r="AB45" s="73"/>
-      <c r="AC45" s="73"/>
-      <c r="AD45" s="73"/>
-      <c r="AE45" s="73"/>
-      <c r="AF45" s="73"/>
-      <c r="AG45" s="73"/>
-      <c r="AH45" s="73"/>
-      <c r="AT45" s="44"/>
-      <c r="AU45" s="44"/>
+      <c r="C45" s="64"/>
+      <c r="D45" s="68"/>
+      <c r="E45" s="68"/>
+      <c r="F45" s="68"/>
+      <c r="G45" s="68"/>
+      <c r="H45" s="68"/>
+      <c r="I45" s="68"/>
+      <c r="J45" s="68"/>
+      <c r="K45" s="68"/>
+      <c r="L45" s="68"/>
+      <c r="M45" s="68"/>
+      <c r="N45" s="68"/>
+      <c r="O45" s="68"/>
+      <c r="P45" s="68"/>
+      <c r="Q45" s="68"/>
+      <c r="R45" s="68"/>
+      <c r="S45" s="68"/>
+      <c r="T45" s="68"/>
+      <c r="U45" s="68"/>
+      <c r="V45" s="68"/>
+      <c r="W45" s="68"/>
+      <c r="X45" s="68"/>
+      <c r="Y45" s="68"/>
+      <c r="Z45" s="68"/>
+      <c r="AA45" s="68"/>
+      <c r="AB45" s="68"/>
+      <c r="AC45" s="68"/>
+      <c r="AD45" s="68"/>
+      <c r="AE45" s="68"/>
+      <c r="AF45" s="68"/>
+      <c r="AG45" s="68"/>
+      <c r="AH45" s="68"/>
       <c r="AV45" s="40"/>
-      <c r="AW45" s="44"/>
     </row>
     <row r="46" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="32"/>
       <c r="B46" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="69"/>
+      <c r="C46" s="64"/>
       <c r="D46" s="25"/>
       <c r="E46" s="25"/>
       <c r="F46" s="25"/>
-      <c r="G46" s="73"/>
-      <c r="H46" s="73"/>
-      <c r="I46" s="73"/>
-      <c r="J46" s="73"/>
-      <c r="K46" s="73"/>
-      <c r="L46" s="73"/>
-      <c r="M46" s="73"/>
-      <c r="N46" s="73"/>
-      <c r="O46" s="73"/>
-      <c r="P46" s="73"/>
-      <c r="Q46" s="73"/>
-      <c r="R46" s="73"/>
-      <c r="S46" s="73"/>
-      <c r="T46" s="73"/>
-      <c r="U46" s="73"/>
-      <c r="V46" s="73"/>
-      <c r="W46" s="73"/>
-      <c r="X46" s="73"/>
-      <c r="Y46" s="73"/>
-      <c r="Z46" s="73"/>
-      <c r="AA46" s="73"/>
-      <c r="AB46" s="73"/>
-      <c r="AC46" s="73"/>
-      <c r="AD46" s="73"/>
-      <c r="AE46" s="73"/>
-      <c r="AF46" s="73"/>
-      <c r="AG46" s="73"/>
-      <c r="AH46" s="73"/>
-      <c r="AT46" s="44"/>
-      <c r="AU46" s="44"/>
+      <c r="G46" s="68"/>
+      <c r="H46" s="68"/>
+      <c r="I46" s="68"/>
+      <c r="J46" s="68"/>
+      <c r="K46" s="68"/>
+      <c r="L46" s="68"/>
+      <c r="M46" s="68"/>
+      <c r="N46" s="68"/>
+      <c r="O46" s="68"/>
+      <c r="P46" s="68"/>
+      <c r="Q46" s="68"/>
+      <c r="R46" s="68"/>
+      <c r="S46" s="68"/>
+      <c r="T46" s="68"/>
+      <c r="U46" s="68"/>
+      <c r="V46" s="68"/>
+      <c r="W46" s="68"/>
+      <c r="X46" s="68"/>
+      <c r="Y46" s="68"/>
+      <c r="Z46" s="68"/>
+      <c r="AA46" s="68"/>
+      <c r="AB46" s="68"/>
+      <c r="AC46" s="68"/>
+      <c r="AD46" s="68"/>
+      <c r="AE46" s="68"/>
+      <c r="AF46" s="68"/>
+      <c r="AG46" s="68"/>
+      <c r="AH46" s="68"/>
       <c r="AV46" s="40"/>
-      <c r="AW46" s="44"/>
     </row>
     <row r="47" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="32"/>
       <c r="B47" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="69"/>
+      <c r="C47" s="64"/>
       <c r="D47" s="25"/>
       <c r="E47" s="25"/>
       <c r="F47" s="25"/>
       <c r="G47" s="25"/>
       <c r="H47" s="25"/>
       <c r="I47" s="25"/>
-      <c r="J47" s="73"/>
-      <c r="K47" s="73"/>
-      <c r="L47" s="73"/>
-      <c r="M47" s="73"/>
-      <c r="N47" s="73"/>
-      <c r="O47" s="73"/>
-      <c r="P47" s="73"/>
-      <c r="Q47" s="73"/>
-      <c r="R47" s="73"/>
-      <c r="S47" s="73"/>
-      <c r="T47" s="73"/>
-      <c r="U47" s="73"/>
-      <c r="V47" s="73"/>
-      <c r="W47" s="73"/>
-      <c r="X47" s="73"/>
-      <c r="Y47" s="73"/>
-      <c r="Z47" s="73"/>
-      <c r="AA47" s="73"/>
-      <c r="AB47" s="73"/>
-      <c r="AC47" s="73"/>
-      <c r="AD47" s="73"/>
-      <c r="AE47" s="73"/>
-      <c r="AF47" s="73"/>
-      <c r="AG47" s="73"/>
-      <c r="AH47" s="73"/>
-      <c r="AT47" s="44"/>
-      <c r="AU47" s="44"/>
+      <c r="J47" s="68"/>
+      <c r="K47" s="68"/>
+      <c r="L47" s="68"/>
+      <c r="M47" s="68"/>
+      <c r="N47" s="68"/>
+      <c r="O47" s="68"/>
+      <c r="P47" s="68"/>
+      <c r="Q47" s="68"/>
+      <c r="R47" s="68"/>
+      <c r="S47" s="68"/>
+      <c r="T47" s="68"/>
+      <c r="U47" s="68"/>
+      <c r="V47" s="68"/>
+      <c r="W47" s="68"/>
+      <c r="X47" s="68"/>
+      <c r="Y47" s="68"/>
+      <c r="Z47" s="68"/>
+      <c r="AA47" s="68"/>
+      <c r="AB47" s="68"/>
+      <c r="AC47" s="68"/>
+      <c r="AD47" s="68"/>
+      <c r="AE47" s="68"/>
+      <c r="AF47" s="68"/>
+      <c r="AG47" s="68"/>
+      <c r="AH47" s="68"/>
       <c r="AV47" s="40"/>
-      <c r="AW47" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="18">

</xml_diff>